<commit_message>
[Taskv10] v2 Make graph for Road Intersection Network/Graph.
	- Changes in street.xlsx.
	- initial map, showing all streets.
</commit_message>
<xml_diff>
--- a/street.xlsx
+++ b/street.xlsx
@@ -144,7 +144,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000000"/>
+  </numFmts>
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,12 +281,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -634,14 +631,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1000,7 +996,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,447 +1007,447 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>123.847311</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>10.27159</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>123.87074200000001</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>10.289747</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>123.870442</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>10.301443000000001</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>123.876278</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>10.290338</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>123.877695</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>10.290634000000001</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>123.87898199999999</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>10.299543</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>123.88799400000001</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>10.297136</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>123.881085</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>10.329267</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>123.885634</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>10.315671999999999</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>123.886707</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>10.307819</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>123.888381</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="3">
         <v>10.297221</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="3">
         <v>123.89692100000001</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <v>10.299459000000001</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="3">
         <v>123.89829400000001</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="3">
         <v>10.296165</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="3">
         <v>123.90606200000001</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="3">
         <v>10.29397</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="3">
         <v>123.90509400000001</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="3">
         <v>10.294419</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="3">
         <v>123.893445</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="3">
         <v>10.309086000000001</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C18">
-        <v>123.886707</v>
-      </c>
-      <c r="D18">
-        <v>10.307819</v>
+      <c r="C18" s="3">
+        <v>123.892629</v>
+      </c>
+      <c r="D18" s="3">
+        <v>10.309339</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="3">
         <v>123.892887</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="3">
         <v>10.310479000000001</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="3">
         <v>123.893917</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="3">
         <v>10.309803</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="3">
         <v>123.89095500000001</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="3">
         <v>10.316094</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="3">
         <v>123.90001100000001</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="3">
         <v>10.318459000000001</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="3">
         <v>123.901684</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="3">
         <v>10.315461000000001</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="3">
         <v>123.903873</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="3">
         <v>10.310732</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="2">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="3">
         <v>123.907135</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="3">
         <v>10.30879</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="3">
         <v>123.909924</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="3">
         <v>10.307100999999999</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" s="2">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="3">
         <v>123.912756</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="3">
         <v>10.303597</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" s="2">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="3">
         <v>123.919151</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="3">
         <v>10.308832000000001</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" s="2">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="3">
         <v>123.91623300000001</v>
       </c>
-      <c r="D29">
-        <v>10.308832000000001</v>
+      <c r="D29" s="3">
+        <v>10.312294</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="A30" s="2">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="3">
         <v>123.914688</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="3">
         <v>10.314194000000001</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" s="2">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="3">
         <v>123.90765</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="3">
         <v>10.325932</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" s="2">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="3">
         <v>123.903873</v>
       </c>
       <c r="D32" s="1">
@@ -1459,44 +1455,44 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" s="2">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="3">
         <v>123.923957</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="3">
         <v>10.371568999999999</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="A34" s="2">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="3">
         <v>123.856403</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="3">
         <v>10.270092</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="A35" s="2">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="1">
         <v>123.89816500000001</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="3">
         <v>10.330997999999999</v>
       </c>
     </row>

</xml_diff>